<commit_message>
refactored the code. stimulus selection according to typicality bins.
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2/input_files/1_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2/input_files/1_scenecat_block_order.xlsx
@@ -1,46 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <workbookPr date1904="false"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t xml:space="preserve">living_room_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kitchen_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">living_room_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kitchen_2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedroom_1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bedroom_2</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,13 +52,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
@@ -122,6 +112,10 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -147,12 +141,15 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
         <a:font script="Thai" typeface="Tahoma"/>
@@ -178,7 +175,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -354,155 +350,166 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="true"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>kitchens_1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>living_rooms_1</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>bedrooms_1</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>kitchens_2</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>bedrooms_2</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>living_rooms_2</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="n">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
         <v>1</v>
       </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="n">
-        <v>0</v>
-      </c>
-      <c r="F2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="n">
-        <v>0</v>
-      </c>
-      <c r="B3" t="n">
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
         <v>1</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
-      <c r="D3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>0</v>
-      </c>
-      <c r="B4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C4" t="n">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
         <v>1</v>
       </c>
-      <c r="D4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>0</v>
-      </c>
-      <c r="B5" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
-      <c r="D5" t="n">
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
         <v>1</v>
       </c>
-      <c r="E5" t="n">
-        <v>0</v>
-      </c>
-      <c r="F5" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>0</v>
-      </c>
-      <c r="B6" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>0</v>
-      </c>
-      <c r="D6" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1</v>
-      </c>
-      <c r="F6" t="n">
+      <c r="F6">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>0</v>
-      </c>
-      <c r="B7" t="n">
-        <v>0</v>
-      </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" t="n">
+      <c r="A7">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
         <v>1</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
rewriting input list generator to make sure all subjs get same selection of imgs.
</commit_message>
<xml_diff>
--- a/scene_cat_exp_2023.2/input_files/1_scenecat_block_order.xlsx
+++ b/scene_cat_exp_2023.2/input_files/1_scenecat_block_order.xlsx
@@ -360,27 +360,27 @@
     <row r="1" s="1" customFormat="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>bedrooms_1</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>kitchens_1</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>living_rooms_1</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>bedrooms_1</t>
-        </is>
-      </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>kitchens_2</t>
+          <t>bedrooms_2</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>bedrooms_2</t>
+          <t>kitchens_2</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">

</xml_diff>